<commit_message>
manual_tracking funciona version basica
</commit_message>
<xml_diff>
--- a/AlejandroAlonso/results/tracking_3_test.xlsx
+++ b/AlejandroAlonso/results/tracking_3_test.xlsx
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -498,11 +498,6 @@
           <t>Bola num 3</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Bola num 4</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="B2" t="inlineStr">
@@ -535,38 +530,28 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>X</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>516</v>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>1251</v>
       </c>
       <c r="D3" t="n">
-        <v>200</v>
+        <v>665</v>
       </c>
       <c r="E3" t="n">
-        <v>200</v>
+        <v>1223</v>
       </c>
       <c r="F3" t="n">
-        <v>300</v>
+        <v>530</v>
       </c>
       <c r="G3" t="n">
-        <v>300</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="4">
@@ -574,22 +559,22 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>105</v>
+        <v>515</v>
       </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>1250</v>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>663</v>
       </c>
       <c r="E4" t="n">
-        <v>200</v>
+        <v>1216</v>
       </c>
       <c r="F4" t="n">
-        <v>300</v>
+        <v>527</v>
       </c>
       <c r="G4" t="n">
-        <v>100</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="5">
@@ -597,37 +582,1473 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>110</v>
+        <v>515</v>
       </c>
       <c r="C5" t="n">
+        <v>1250</v>
+      </c>
+      <c r="D5" t="n">
+        <v>660</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1201</v>
+      </c>
+      <c r="F5" t="n">
+        <v>526</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>516</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1252</v>
+      </c>
+      <c r="D6" t="n">
+        <v>657</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1185</v>
+      </c>
+      <c r="F6" t="n">
+        <v>529</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>516</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1255</v>
+      </c>
+      <c r="D7" t="n">
+        <v>656</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1169</v>
+      </c>
+      <c r="F7" t="n">
+        <v>528</v>
+      </c>
+      <c r="G7" t="n">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>515</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1258</v>
+      </c>
+      <c r="D8" t="n">
+        <v>656</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1154</v>
+      </c>
+      <c r="F8" t="n">
+        <v>527</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>522</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1254</v>
+      </c>
+      <c r="D9" t="n">
+        <v>657</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1141</v>
+      </c>
+      <c r="F9" t="n">
+        <v>534</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1217</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>528</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1241</v>
+      </c>
+      <c r="D10" t="n">
+        <v>658</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1133</v>
+      </c>
+      <c r="F10" t="n">
+        <v>537</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1213</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>533</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1218</v>
+      </c>
+      <c r="D11" t="n">
+        <v>661</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1136</v>
+      </c>
+      <c r="F11" t="n">
+        <v>541</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1195</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>678</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1164</v>
+      </c>
+      <c r="D12" t="n">
+        <v>665</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1143</v>
+      </c>
+      <c r="F12" t="n">
+        <v>547</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1162</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>543</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1146</v>
+      </c>
+      <c r="D13" t="n">
+        <v>666</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1153</v>
+      </c>
+      <c r="F13" t="n">
+        <v>551</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1127</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>547</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1075</v>
+      </c>
+      <c r="D14" t="n">
+        <v>666</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1164</v>
+      </c>
+      <c r="F14" t="n">
+        <v>549</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>550</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1011</v>
+      </c>
+      <c r="D15" t="n">
+        <v>662</v>
+      </c>
+      <c r="E15" t="n">
+        <v>1173</v>
+      </c>
+      <c r="F15" t="n">
+        <v>547</v>
+      </c>
+      <c r="G15" t="n">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>554</v>
+      </c>
+      <c r="C16" t="n">
+        <v>967</v>
+      </c>
+      <c r="D16" t="n">
+        <v>659</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1184</v>
+      </c>
+      <c r="F16" t="n">
+        <v>545</v>
+      </c>
+      <c r="G16" t="n">
+        <v>1044</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
         <v>15</v>
       </c>
-      <c r="D5" t="n">
-        <v>200</v>
-      </c>
-      <c r="E5" t="n">
-        <v>100</v>
-      </c>
-      <c r="F5" t="n">
-        <v>100</v>
-      </c>
-      <c r="G5" t="n">
-        <v>300</v>
-      </c>
-      <c r="H5" t="n">
-        <v>400</v>
-      </c>
-      <c r="I5" t="n">
-        <v>400</v>
+      <c r="B17" t="n">
+        <v>561</v>
+      </c>
+      <c r="C17" t="n">
+        <v>931</v>
+      </c>
+      <c r="D17" t="n">
+        <v>657</v>
+      </c>
+      <c r="E17" t="n">
+        <v>1197</v>
+      </c>
+      <c r="F17" t="n">
+        <v>542</v>
+      </c>
+      <c r="G17" t="n">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>566</v>
+      </c>
+      <c r="C18" t="n">
+        <v>896</v>
+      </c>
+      <c r="D18" t="n">
+        <v>651</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1204</v>
+      </c>
+      <c r="F18" t="n">
+        <v>539</v>
+      </c>
+      <c r="G18" t="n">
+        <v>1026</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>571</v>
+      </c>
+      <c r="C19" t="n">
+        <v>864</v>
+      </c>
+      <c r="D19" t="n">
+        <v>648</v>
+      </c>
+      <c r="E19" t="n">
+        <v>1214</v>
+      </c>
+      <c r="F19" t="n">
+        <v>537</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>577</v>
+      </c>
+      <c r="C20" t="n">
+        <v>833</v>
+      </c>
+      <c r="D20" t="n">
+        <v>645</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1224</v>
+      </c>
+      <c r="F20" t="n">
+        <v>534</v>
+      </c>
+      <c r="G20" t="n">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>585</v>
+      </c>
+      <c r="C21" t="n">
+        <v>808</v>
+      </c>
+      <c r="D21" t="n">
+        <v>642</v>
+      </c>
+      <c r="E21" t="n">
+        <v>1229</v>
+      </c>
+      <c r="F21" t="n">
+        <v>531</v>
+      </c>
+      <c r="G21" t="n">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>593</v>
+      </c>
+      <c r="C22" t="n">
+        <v>793</v>
+      </c>
+      <c r="D22" t="n">
+        <v>639</v>
+      </c>
+      <c r="E22" t="n">
+        <v>1223</v>
+      </c>
+      <c r="F22" t="n">
+        <v>528</v>
+      </c>
+      <c r="G22" t="n">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>603</v>
+      </c>
+      <c r="C23" t="n">
+        <v>789</v>
+      </c>
+      <c r="D23" t="n">
+        <v>630</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1206</v>
+      </c>
+      <c r="F23" t="n">
+        <v>529</v>
+      </c>
+      <c r="G23" t="n">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>610</v>
+      </c>
+      <c r="C24" t="n">
+        <v>782</v>
+      </c>
+      <c r="D24" t="n">
+        <v>619</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1184</v>
+      </c>
+      <c r="F24" t="n">
+        <v>528</v>
+      </c>
+      <c r="G24" t="n">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>618</v>
+      </c>
+      <c r="C25" t="n">
+        <v>781</v>
+      </c>
+      <c r="D25" t="n">
+        <v>608</v>
+      </c>
+      <c r="E25" t="n">
+        <v>1156</v>
+      </c>
+      <c r="F25" t="n">
+        <v>525</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1113</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>624</v>
+      </c>
+      <c r="C26" t="n">
+        <v>789</v>
+      </c>
+      <c r="D26" t="n">
+        <v>597</v>
+      </c>
+      <c r="E26" t="n">
+        <v>1115</v>
+      </c>
+      <c r="F26" t="n">
+        <v>524</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>630</v>
+      </c>
+      <c r="C27" t="n">
+        <v>803</v>
+      </c>
+      <c r="D27" t="n">
+        <v>587</v>
+      </c>
+      <c r="E27" t="n">
+        <v>1067</v>
+      </c>
+      <c r="F27" t="n">
+        <v>523</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>638</v>
+      </c>
+      <c r="C28" t="n">
+        <v>823</v>
+      </c>
+      <c r="D28" t="n">
+        <v>581</v>
+      </c>
+      <c r="E28" t="n">
+        <v>1016</v>
+      </c>
+      <c r="F28" t="n">
+        <v>522</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1171</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>649</v>
+      </c>
+      <c r="C29" t="n">
+        <v>845</v>
+      </c>
+      <c r="D29" t="n">
+        <v>574</v>
+      </c>
+      <c r="E29" t="n">
+        <v>970</v>
+      </c>
+      <c r="F29" t="n">
+        <v>522</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>659</v>
+      </c>
+      <c r="C30" t="n">
+        <v>874</v>
+      </c>
+      <c r="D30" t="n">
+        <v>566</v>
+      </c>
+      <c r="E30" t="n">
+        <v>938</v>
+      </c>
+      <c r="F30" t="n">
+        <v>526</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1209</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>668</v>
+      </c>
+      <c r="C31" t="n">
+        <v>908</v>
+      </c>
+      <c r="D31" t="n">
+        <v>558</v>
+      </c>
+      <c r="E31" t="n">
+        <v>910</v>
+      </c>
+      <c r="F31" t="n">
+        <v>529</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1227</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>676</v>
+      </c>
+      <c r="C32" t="n">
+        <v>947</v>
+      </c>
+      <c r="D32" t="n">
+        <v>551</v>
+      </c>
+      <c r="E32" t="n">
+        <v>880</v>
+      </c>
+      <c r="F32" t="n">
+        <v>532</v>
+      </c>
+      <c r="G32" t="n">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>684</v>
+      </c>
+      <c r="C33" t="n">
+        <v>986</v>
+      </c>
+      <c r="D33" t="n">
+        <v>545</v>
+      </c>
+      <c r="E33" t="n">
+        <v>851</v>
+      </c>
+      <c r="F33" t="n">
+        <v>538</v>
+      </c>
+      <c r="G33" t="n">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>694</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1016</v>
+      </c>
+      <c r="D34" t="n">
+        <v>536</v>
+      </c>
+      <c r="E34" t="n">
+        <v>840</v>
+      </c>
+      <c r="F34" t="n">
+        <v>546</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1220</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>702</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1034</v>
+      </c>
+      <c r="D35" t="n">
+        <v>531</v>
+      </c>
+      <c r="E35" t="n">
+        <v>829</v>
+      </c>
+      <c r="F35" t="n">
+        <v>556</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>709</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1050</v>
+      </c>
+      <c r="D36" t="n">
+        <v>527</v>
+      </c>
+      <c r="E36" t="n">
+        <v>825</v>
+      </c>
+      <c r="F36" t="n">
+        <v>568</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>711</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1072</v>
+      </c>
+      <c r="D37" t="n">
+        <v>522</v>
+      </c>
+      <c r="E37" t="n">
+        <v>828</v>
+      </c>
+      <c r="F37" t="n">
+        <v>580</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1148</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>710</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1096</v>
+      </c>
+      <c r="D38" t="n">
+        <v>517</v>
+      </c>
+      <c r="E38" t="n">
+        <v>833</v>
+      </c>
+      <c r="F38" t="n">
+        <v>590</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>699</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1117</v>
+      </c>
+      <c r="D39" t="n">
+        <v>512</v>
+      </c>
+      <c r="E39" t="n">
+        <v>842</v>
+      </c>
+      <c r="F39" t="n">
+        <v>590</v>
+      </c>
+      <c r="G39" t="n">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>691</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1136</v>
+      </c>
+      <c r="D40" t="n">
+        <v>508</v>
+      </c>
+      <c r="E40" t="n">
+        <v>863</v>
+      </c>
+      <c r="F40" t="n">
+        <v>591</v>
+      </c>
+      <c r="G40" t="n">
+        <v>976</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>684</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1150</v>
+      </c>
+      <c r="D41" t="n">
+        <v>503</v>
+      </c>
+      <c r="E41" t="n">
+        <v>891</v>
+      </c>
+      <c r="F41" t="n">
+        <v>592</v>
+      </c>
+      <c r="G41" t="n">
+        <v>931</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="D42" t="n">
+        <v>498</v>
+      </c>
+      <c r="E42" t="n">
+        <v>920</v>
+      </c>
+      <c r="F42" t="n">
+        <v>593</v>
+      </c>
+      <c r="G42" t="n">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>670</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1179</v>
+      </c>
+      <c r="D43" t="n">
+        <v>495</v>
+      </c>
+      <c r="E43" t="n">
+        <v>952</v>
+      </c>
+      <c r="F43" t="n">
+        <v>594</v>
+      </c>
+      <c r="G43" t="n">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>663</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1194</v>
+      </c>
+      <c r="D44" t="n">
+        <v>494</v>
+      </c>
+      <c r="E44" t="n">
+        <v>985</v>
+      </c>
+      <c r="F44" t="n">
+        <v>595</v>
+      </c>
+      <c r="G44" t="n">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>657</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1209</v>
+      </c>
+      <c r="D45" t="n">
+        <v>493</v>
+      </c>
+      <c r="E45" t="n">
+        <v>1018</v>
+      </c>
+      <c r="F45" t="n">
+        <v>597</v>
+      </c>
+      <c r="G45" t="n">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>650</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1218</v>
+      </c>
+      <c r="D46" t="n">
+        <v>485</v>
+      </c>
+      <c r="E46" t="n">
+        <v>1034</v>
+      </c>
+      <c r="F46" t="n">
+        <v>597</v>
+      </c>
+      <c r="G46" t="n">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>640</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1212</v>
+      </c>
+      <c r="D47" t="n">
+        <v>479</v>
+      </c>
+      <c r="E47" t="n">
+        <v>1050</v>
+      </c>
+      <c r="F47" t="n">
+        <v>597</v>
+      </c>
+      <c r="G47" t="n">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>634</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1210</v>
+      </c>
+      <c r="D48" t="n">
+        <v>478</v>
+      </c>
+      <c r="E48" t="n">
+        <v>1061</v>
+      </c>
+      <c r="F48" t="n">
+        <v>603</v>
+      </c>
+      <c r="G48" t="n">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>624</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1201</v>
+      </c>
+      <c r="D49" t="n">
+        <v>481</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1069</v>
+      </c>
+      <c r="F49" t="n">
+        <v>610</v>
+      </c>
+      <c r="G49" t="n">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>613</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1186</v>
+      </c>
+      <c r="D50" t="n">
+        <v>483</v>
+      </c>
+      <c r="E50" t="n">
+        <v>1085</v>
+      </c>
+      <c r="F50" t="n">
+        <v>614</v>
+      </c>
+      <c r="G50" t="n">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>600</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D51" t="n">
+        <v>485</v>
+      </c>
+      <c r="E51" t="n">
+        <v>1105</v>
+      </c>
+      <c r="F51" t="n">
+        <v>616</v>
+      </c>
+      <c r="G51" t="n">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>588</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D52" t="n">
+        <v>489</v>
+      </c>
+      <c r="E52" t="n">
+        <v>1125</v>
+      </c>
+      <c r="F52" t="n">
+        <v>618</v>
+      </c>
+      <c r="G52" t="n">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>580</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1045</v>
+      </c>
+      <c r="D53" t="n">
+        <v>493</v>
+      </c>
+      <c r="E53" t="n">
+        <v>1145</v>
+      </c>
+      <c r="F53" t="n">
+        <v>623</v>
+      </c>
+      <c r="G53" t="n">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>576</v>
+      </c>
+      <c r="C54" t="n">
+        <v>991</v>
+      </c>
+      <c r="D54" t="n">
+        <v>496</v>
+      </c>
+      <c r="E54" t="n">
+        <v>1165</v>
+      </c>
+      <c r="F54" t="n">
+        <v>628</v>
+      </c>
+      <c r="G54" t="n">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>572</v>
+      </c>
+      <c r="C55" t="n">
+        <v>946</v>
+      </c>
+      <c r="D55" t="n">
+        <v>496</v>
+      </c>
+      <c r="E55" t="n">
+        <v>1186</v>
+      </c>
+      <c r="F55" t="n">
+        <v>633</v>
+      </c>
+      <c r="G55" t="n">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>569</v>
+      </c>
+      <c r="C56" t="n">
+        <v>911</v>
+      </c>
+      <c r="D56" t="n">
+        <v>497</v>
+      </c>
+      <c r="E56" t="n">
+        <v>1205</v>
+      </c>
+      <c r="F56" t="n">
+        <v>638</v>
+      </c>
+      <c r="G56" t="n">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>565</v>
+      </c>
+      <c r="C57" t="n">
+        <v>887</v>
+      </c>
+      <c r="D57" t="n">
+        <v>500</v>
+      </c>
+      <c r="E57" t="n">
+        <v>1221</v>
+      </c>
+      <c r="F57" t="n">
+        <v>643</v>
+      </c>
+      <c r="G57" t="n">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>559</v>
+      </c>
+      <c r="C58" t="n">
+        <v>857</v>
+      </c>
+      <c r="D58" t="n">
+        <v>504</v>
+      </c>
+      <c r="E58" t="n">
+        <v>1234</v>
+      </c>
+      <c r="F58" t="n">
+        <v>648</v>
+      </c>
+      <c r="G58" t="n">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>550</v>
+      </c>
+      <c r="C59" t="n">
+        <v>826</v>
+      </c>
+      <c r="D59" t="n">
+        <v>509</v>
+      </c>
+      <c r="E59" t="n">
+        <v>1241</v>
+      </c>
+      <c r="F59" t="n">
+        <v>660</v>
+      </c>
+      <c r="G59" t="n">
+        <v>974</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>548</v>
+      </c>
+      <c r="C60" t="n">
+        <v>815</v>
+      </c>
+      <c r="D60" t="n">
+        <v>518</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1238</v>
+      </c>
+      <c r="F60" t="n">
+        <v>671</v>
+      </c>
+      <c r="G60" t="n">
+        <v>983</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>542</v>
+      </c>
+      <c r="C61" t="n">
+        <v>803</v>
+      </c>
+      <c r="D61" t="n">
+        <v>535</v>
+      </c>
+      <c r="E61" t="n">
+        <v>1226</v>
+      </c>
+      <c r="F61" t="n">
+        <v>675</v>
+      </c>
+      <c r="G61" t="n">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>540</v>
+      </c>
+      <c r="C62" t="n">
+        <v>796</v>
+      </c>
+      <c r="D62" t="n">
+        <v>553</v>
+      </c>
+      <c r="E62" t="n">
+        <v>1208</v>
+      </c>
+      <c r="F62" t="n">
+        <v>681</v>
+      </c>
+      <c r="G62" t="n">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>536</v>
+      </c>
+      <c r="C63" t="n">
+        <v>798</v>
+      </c>
+      <c r="D63" t="n">
+        <v>568</v>
+      </c>
+      <c r="E63" t="n">
+        <v>1182</v>
+      </c>
+      <c r="F63" t="n">
+        <v>687</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>532</v>
+      </c>
+      <c r="C64" t="n">
+        <v>813</v>
+      </c>
+      <c r="D64" t="n">
+        <v>580</v>
+      </c>
+      <c r="E64" t="n">
+        <v>1148</v>
+      </c>
+      <c r="F64" t="n">
+        <v>692</v>
+      </c>
+      <c r="G64" t="n">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>529</v>
+      </c>
+      <c r="C65" t="n">
+        <v>823</v>
+      </c>
+      <c r="D65" t="n">
+        <v>585</v>
+      </c>
+      <c r="E65" t="n">
+        <v>1091</v>
+      </c>
+      <c r="F65" t="n">
+        <v>696</v>
+      </c>
+      <c r="G65" t="n">
+        <v>1062</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>527</v>
+      </c>
+      <c r="C66" t="n">
+        <v>839</v>
+      </c>
+      <c r="D66" t="n">
+        <v>590</v>
+      </c>
+      <c r="E66" t="n">
+        <v>1034</v>
+      </c>
+      <c r="F66" t="n">
+        <v>696</v>
+      </c>
+      <c r="G66" t="n">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>527</v>
+      </c>
+      <c r="C67" t="n">
+        <v>863</v>
+      </c>
+      <c r="D67" t="n">
+        <v>593</v>
+      </c>
+      <c r="E67" t="n">
+        <v>978</v>
+      </c>
+      <c r="F67" t="n">
+        <v>696</v>
+      </c>
+      <c r="G67" t="n">
+        <v>1106</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>525</v>
+      </c>
+      <c r="C68" t="n">
+        <v>891</v>
+      </c>
+      <c r="D68" t="n">
+        <v>596</v>
+      </c>
+      <c r="E68" t="n">
+        <v>931</v>
+      </c>
+      <c r="F68" t="n">
+        <v>699</v>
+      </c>
+      <c r="G68" t="n">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>